<commit_message>
setting up code for NN
</commit_message>
<xml_diff>
--- a/data/df_false_pos.xlsx
+++ b/data/df_false_pos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,7 +469,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>bond outings recent years , stunts outlandish border cartoonlike . heavy reliance cgi technology beginning creep series .</t>
+          <t>bond outings recent years stunts outlandish border cartoonlike heavy reliance cgi technology beginning creep series</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -490,7 +490,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>part charm satin rouge avoids obvious humour lightness .</t>
+          <t>part charm satin rouge avoids obvious humour lightness</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -511,7 +511,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>mysteries transparently obvious , 's slowly paced thriller . [ 's ] worth recommending two marvelous performances michael caine brendan fraser .</t>
+          <t>mysteries transparently obvious slowly paced thriller worth recommending two marvelous performances michael caine brendan fraser</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -532,7 +532,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>maybe 's past year seen release worst comedies decades . . . honestly , analyze really n't bad .</t>
+          <t>maybe past year seen release worst comedies decades honestly analyze really isnt bad</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -553,7 +553,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>polished korean political-action -- bad -- hollywood action epics . progress ?</t>
+          <t>polished korean politicalaction bad hollywood action epics progress</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -574,7 +574,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>could say 's slow times , could say characters act ways real people would n't , thing could n't say alias betty predictable .</t>
+          <t>could say slow times could say characters act ways real people wouldnt thing couldnt say alias betty predictable</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -595,7 +595,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>asia authors anna battista , italian superstar aspiring directress happens worst enemy .</t>
+          <t>asia authors anna battista italian superstar aspiring directress happens worst enemy</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -616,7 +616,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>least surprising , still ultimately satisfying . think sort comfort food mind .</t>
+          <t>least surprising still ultimately satisfying think sort comfort food mind</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -637,7 +637,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>hour photo intriguing snapshot man delusions ; 's bad n't flashes insight .</t>
+          <t>hour photo intriguing snapshot man delusions bad doesnt flashes insight</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -658,7 +658,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>whole cast looks fun slapstick antics silly street patois , tossing around obscure expressions bellini mullinski , compact 86 minutes breezes .</t>
+          <t>whole cast looks fun slapstick antics silly street patois tossing around obscure expressions bellini mullinski compact minutes breezes</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -679,7 +679,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>still pretentious filled subtext , entertaining 'face value ' recommend anyone looking something different .</t>
+          <t>still pretentious filled subtext entertaining face value recommend anyone looking something different</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -700,7 +700,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>message seems facile earlier films , images terrible beauty may care .</t>
+          <t>message seems facile earlier films images terrible beauty may care</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -721,7 +721,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>story feels serious read , filled heavy doses always enticing sayles dialogue .</t>
+          <t>story feels serious read filled heavy doses always enticing sayles dialogue</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -742,7 +742,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[ herzog 's ] least inspired works .</t>
+          <t>herzogs least inspired works</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>boisterous comedy serves cruel reminder fate hundreds thousands chinese , qualify terrible tragedy .</t>
+          <t>boisterous comedy serves cruel reminder fate hundreds thousands chinese qualify terrible tragedy</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -784,7 +784,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>provide [ ] nail-biting suspense credible characters without relying technology-of-the-moment technique pretentious dialogue .</t>
+          <t>provides nailbiting suspense credible characters without relying technologyofthemoment technique pretentious dialogue</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -805,7 +805,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>sure , 's , proves , 's always bad thing .</t>
+          <t>sure proves thats always bad thing</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -826,7 +826,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>smith 's point simple obvious -- people 's homes extensions , particularly eccentric people particularly eccentric living spaces -- subjects charmers .</t>
+          <t>smiths point simple obvious peoples homes extensions particularly eccentric people particularly eccentric living spaces subjects charmers</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -847,7 +847,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>time changer may memorable cinema session profound self-evaluation message fragile existence absence spiritual guidance least invade abundance mindsets</t>
+          <t>time changer may memorable cinema session profound selfevaluation message fragile existence absence spiritual guidance least invade abundance mindsets</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -868,7 +868,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>`` emperor 's new clothes `` begins simple plan . . . . well , least 's plan .</t>
+          <t>emperors new clothes begins simple plan well least thats plan</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -889,7 +889,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>despite story predictable sound music play nail-biting thriller , heart right place difficult get really peeved .</t>
+          <t>despite story predictable sound music play nailbiting thriller heart right place difficult get really peeved</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -910,7 +910,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>happy throwback time cartoons cinema 's idiosyncratic form instead predictable .</t>
+          <t>happy throwback time cartoons cinemas idiosyncratic form instead predictable</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -931,7 +931,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>light , silly , photographed colour depth , rather time .</t>
+          <t>light silly photographed colour depth rather time</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -952,7 +952,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>courage wonder big questions sincerity devotion . risks seeming slow pretentious , thinks gamble worth promise .</t>
+          <t>courage wonder big questions sincerity devotion risks seeming slow pretentious thinks gamble worth promise</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -973,7 +973,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>though plot predictable , never feels formulaic , attention nuances emotional development delicate characters .</t>
+          <t>though plot predictable never feels formulaic attention nuances emotional development delicate characters</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -994,7 +994,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>'s predictable , jumps expected hoops style even depth .</t>
+          <t>predictable jumps expected hoops style even depth</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1015,7 +1015,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>mr . zhang 's subject matter , degree least , quintessentially american , approach storytelling might called iranian .</t>
+          <t>mr zhangs subject matter degree least quintessentially american approach storytelling might called iranian</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1024,11 +1024,11 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>857</v>
+        <v>838</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>evokes a little of the fear that parents have for the possible futures of their children--and the sometimes bad choices mothers and fathers make in the interests of doing them good .</t>
+          <t>a sweet-natured reconsideration of one of san francisco's most vital , if least widely recognized , creative fountainheads .</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>evokes fear parents possible futures children -- sometimes bad choices mothers fathers interests .</t>
+          <t>sweetnatured reconsideration san franciscos vital least widely recognized creative fountainheads</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1045,11 +1045,11 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>871</v>
+        <v>857</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>a sly game of cat and mouse that's intense and thrilling at times , but occasionally stretches believability to its limits and relies on predictable plot contrivances .</t>
+          <t>evokes a little of the fear that parents have for the possible futures of their children--and the sometimes bad choices mothers and fathers make in the interests of doing them good .</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1057,7 +1057,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>sly game cat mouse 's intense thrilling times , occasionally stretches believability limits relies predictable plot contrivances .</t>
+          <t>evokes fear parents possible futures childrenand sometimes bad choices mothers fathers interests</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1066,11 +1066,11 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>this horror-comedy doesn't go for the usual obvious laughs at the expense of cheap-looking monsters -- unless you count elvira's hooters .</t>
+          <t>a sly game of cat and mouse that's intense and thrilling at times , but occasionally stretches believability to its limits and relies on predictable plot contrivances .</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>horror-comedy n't go usual obvious laughs expense cheap-looking monsters -- unless count elvira 's hooters .</t>
+          <t>sly game cat mouse thats intense thrilling times occasionally stretches believability limits relies predictable plot contrivances</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1087,11 +1087,11 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>not a bad journey at all .</t>
+          <t>this horror-comedy doesn't go for the usual obvious laughs at the expense of cheap-looking monsters -- unless you count elvira's hooters .</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>bad journey .</t>
+          <t>horrorcomedy doesnt go usual obvious laughs expense cheaplooking monsters unless count elviras hooters</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1108,11 +1108,11 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>925</v>
+        <v>875</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>a love for films shines through each frame and the era is recreated with obvious affection , scored to perfection with some tasty boogaloo beats .</t>
+          <t>not a bad journey at all .</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>love films shines frame era recreated obvious affection , scored perfection tasty boogaloo beats .</t>
+          <t>bad journey</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1129,11 +1129,11 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>933</v>
+        <v>925</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>mixes likeable personalities , inventive photography and cutting , and wall-to-wall toe-tapping music to paint a picture of a subculture that is at once exhilarating , silly , perverse , hopeful and always fun .</t>
+          <t>a love for films shines through each frame and the era is recreated with obvious affection , scored to perfection with some tasty boogaloo beats .</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>mixes likeable personalities , inventive photography cutting , wall-to-wall toe-tapping music paint picture subculture exhilarating , silly , perverse , hopeful always fun .</t>
+          <t>love films shines frame era recreated obvious affection scored perfection tasty boogaloo beats</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1150,11 +1150,11 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>942</v>
+        <v>933</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>it is far from the worst , thanks to the topical issues it raises , the performances of stewart and hardy , and that essential feature -- a decent full-on space battle .</t>
+          <t>mixes likeable personalities , inventive photography and cutting , and wall-to-wall toe-tapping music to paint a picture of a subculture that is at once exhilarating , silly , perverse , hopeful and always fun .</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>far worst , thanks topical issues raises , performances stewart hardy , essential feature -- decent full-on space battle .</t>
+          <t>mixes likeable personalities inventive photography cutting walltowall toetapping music paint picture subculture exhilarating silly perverse hopeful always fun</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1171,11 +1171,11 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>973</v>
+        <v>942</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>never once predictable .</t>
+          <t>it is far from the worst , thanks to the topical issues it raises , the performances of stewart and hardy , and that essential feature -- a decent full-on space battle .</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>never predictable .</t>
+          <t>far worst thanks topical issues raises performances stewart hardy essential feature decent fullon space battle</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1192,11 +1192,11 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>1138</v>
+        <v>973</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>garcía bernal and talancón are an immensely appealing couple , and even though their story is predictable , you'll want things to work out .</t>
+          <t>never once predictable .</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>garcía bernal talancón immensely appealing couple , even though story predictable , 'll want things work .</t>
+          <t>never predictable</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1213,11 +1213,11 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>1183</v>
+        <v>1138</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>' . . . mafia , rap stars and hood rats butt their ugly heads in a regurgitation of cinematic violence that gives brutal birth to an unlikely , but likable , hero . '</t>
+          <t>garcía bernal and talancón are an immensely appealing couple , and even though their story is predictable , you'll want things to work out .</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>' . . . mafia , rap stars hood rats butt ugly heads regurgitation cinematic violence gives brutal birth unlikely , likable , hero . '</t>
+          <t>garca bernal talancn immensely appealing couple even though story predictable youll want things work</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1234,11 +1234,11 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>1189</v>
+        <v>1183</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>even in its most tedious scenes , russian ark is mesmerizing .</t>
+          <t>' . . . mafia , rap stars and hood rats butt their ugly heads in a regurgitation of cinematic violence that gives brutal birth to an unlikely , but likable , hero . '</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>even tedious scenes , russian ark mesmerizing .</t>
+          <t>mafia rap stars hood rats butt ugly heads regurgitation cinematic violence gives brutal birth unlikely likable hero</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1255,11 +1255,11 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>1245</v>
+        <v>1189</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>by the time we learn that andrew's turnabout is fair play is every bit as awful as borchardt's coven , we can enjoy it anyway .</t>
+          <t>even in its most tedious scenes , russian ark is mesmerizing .</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>time learn andrew 's turnabout fair play every bit awful borchardt 's coven , enjoy anyway .</t>
+          <t>even tedious scenes russian ark mesmerizing</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1276,11 +1276,11 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>this riveting world war ii moral suspense story deals with the shadow side of american culture : racial prejudice in its ugly and diverse forms .</t>
+          <t>by the time we learn that andrew's turnabout is fair play is every bit as awful as borchardt's coven , we can enjoy it anyway .</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>riveting world war ii moral suspense story deals shadow side american culture : racial prejudice ugly diverse forms .</t>
+          <t>time learn andrews turnabout fair play every bit awful borchardts coven enjoy anyway</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1297,11 +1297,11 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>1304</v>
+        <v>1246</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>this tenth feature is a big deal , indeed -- at least the third-best , and maybe even a notch above the previous runner-up , nicholas meyer's star trek vi : the undiscovered country .</t>
+          <t>this riveting world war ii moral suspense story deals with the shadow side of american culture : racial prejudice in its ugly and diverse forms .</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>tenth feature big deal , indeed -- least third-best , maybe even notch previous runner-up , nicholas meyer 's star trek vi : undiscovered country .</t>
+          <t>riveting world war ii moral suspense story deals shadow side american culture racial prejudice ugly diverse forms</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1318,11 +1318,11 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>1357</v>
+        <v>1304</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>mr . tsai is a very original artist in his medium , and what time is it there ? should be seen at the very least for its spasms of absurdist humor .</t>
+          <t>this tenth feature is a big deal , indeed -- at least the third-best , and maybe even a notch above the previous runner-up , nicholas meyer's star trek vi : the undiscovered country .</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>mr . tsai original artist medium , time ? seen least spasms absurdist humor .</t>
+          <t>tenth feature big deal indeed least thirdbest maybe even notch previous runnerup nicholas meyers star trek vi undiscovered country</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1339,11 +1339,11 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>1374</v>
+        <v>1357</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>a painfully funny ode to bad behavior .</t>
+          <t>mr . tsai is a very original artist in his medium , and what time is it there ? should be seen at the very least for its spasms of absurdist humor .</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1351,7 +1351,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>painfully ode bad behavior .</t>
+          <t>mr tsai original artist medium time seen least spasms absurdist humor</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -1360,11 +1360,11 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>1467</v>
+        <v>1374</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>the draw [for " big bad love " ] is a solid performance by arliss howard .</t>
+          <t>a painfully funny ode to bad behavior .</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>draw [ `` big bad love `` ] solid performance arliss howard .</t>
+          <t>painfully ode bad behavior</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1381,11 +1381,11 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>1509</v>
+        <v>1467</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>despite its title , punch-drunk love is never heavy-handed . the jabs it employs are short , carefully placed and dead-center .</t>
+          <t>the draw [for " big bad love " ] is a solid performance by arliss howard .</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>despite title , punch-drunk love never heavy-handed . jabs employs short , carefully placed dead-center .</t>
+          <t>draw big bad love solid performance arliss howard</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1414,7 +1414,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>pleasant romance intellectual underpinnings , kind entertains even turns maddeningly predictable .</t>
+          <t>pleasant romance intellectual underpinnings kind entertains even turns maddeningly predictable</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>best silly horror movies recent memory , real shocks store unwary viewers .</t>
+          <t>best silly horror movies recent memory real shocks store unwary viewers</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1444,11 +1444,11 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>1683</v>
+        <v>1767</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>it's the filmmakers' post-camp comprehension of what made old-time b movies good-bad that makes eight legged freaks a perfectly entertaining summer diversion .</t>
+          <t>the result is more depressing than liberating , but it's never boring .</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>'s filmmakers ' post-camp comprehension made old-time b movies good-bad makes eight legged freaks perfectly entertaining summer diversion .</t>
+          <t>result depressing liberating never boring</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1465,11 +1465,11 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>1767</v>
+        <v>1807</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>the result is more depressing than liberating , but it's never boring .</t>
+          <t>predictable storyline and by-the-book scripting is all but washed away by sumptuous ocean visuals and the cinematic stylings of director john stockwell .</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1477,7 +1477,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>result depressing liberating , 's never boring .</t>
+          <t>predictable storyline bythebook scripting washed away sumptuous ocean visuals cinematic stylings director john stockwell</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1486,11 +1486,11 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>1807</v>
+        <v>1817</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>predictable storyline and by-the-book scripting is all but washed away by sumptuous ocean visuals and the cinematic stylings of director john stockwell .</t>
+          <t>high crimes knows the mistakes that bad movies make and is determined not to make them , and maybe that is nobility of a sort .</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1498,7 +1498,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>predictable storyline by-the-book scripting washed away sumptuous ocean visuals cinematic stylings director john stockwell .</t>
+          <t>high crimes knows mistakes bad movies determined maybe nobility sort</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -1507,11 +1507,11 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>1817</v>
+        <v>1862</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>high crimes knows the mistakes that bad movies make and is determined not to make them , and maybe that is nobility of a sort .</t>
+          <t>the film's sense of imagery gives it a terrible strength , but it's propelled by the acting .</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>high crimes knows mistakes bad movies determined , maybe nobility sort .</t>
+          <t>films sense imagery gives terrible strength propelled acting</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -1528,11 +1528,11 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>1862</v>
+        <v>1899</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>the film's sense of imagery gives it a terrible strength , but it's propelled by the acting .</t>
+          <t>well-acted , well-directed and , for all its moodiness , not too pretentious .</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>'s sense imagery gives terrible strength , 's propelled acting .</t>
+          <t>wellacted welldirected moodiness pretentious</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -1549,11 +1549,11 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>1899</v>
+        <v>1902</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>well-acted , well-directed and , for all its moodiness , not too pretentious .</t>
+          <t>real women have curves wears its empowerment on its sleeve but even its worst harangues are easy to swallow thanks to remarkable performances by ferrera and ontiveros .</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>well-acted , well-directed , moodiness , pretentious .</t>
+          <t>real women curves wears empowerment sleeve even worst harangues easy swallow thanks remarkable performances ferrera ontiveros</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -1570,11 +1570,11 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>1902</v>
+        <v>1907</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>real women have curves wears its empowerment on its sleeve but even its worst harangues are easy to swallow thanks to remarkable performances by ferrera and ontiveros .</t>
+          <t>what's so fun about this silly , outrageous , ingenious thriller is the director's talent . watching a brian depalma movie is like watching an alfred hitchcock movie after drinking twelve beers .</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1582,7 +1582,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>real women curves wears empowerment sleeve even worst harangues easy swallow thanks remarkable performances ferrera ontiveros .</t>
+          <t>whats fun silly outrageous ingenious thriller directors talent watching brian depalma watching alfred hitchcock drinking twelve beers</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -1591,11 +1591,11 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>1907</v>
+        <v>1911</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>what's so fun about this silly , outrageous , ingenious thriller is the director's talent . watching a brian depalma movie is like watching an alfred hitchcock movie after drinking twelve beers .</t>
+          <t>this beautifully animated epic is never dull .</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>'s fun silly , outrageous , ingenious thriller director 's talent . watching brian depalma watching alfred hitchcock drinking twelve beers .</t>
+          <t>beautifully animated epic never dull</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -1612,11 +1612,11 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>1911</v>
+        <v>1926</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>this beautifully animated epic is never dull .</t>
+          <t>uplifting as only a document of the worst possibilities of mankind can be , and among the best films of the year .</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>beautifully animated epic never dull .</t>
+          <t>uplifting document worst possibilities mankind among best films year</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -1633,11 +1633,11 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>1926</v>
+        <v>1953</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>uplifting as only a document of the worst possibilities of mankind can be , and among the best films of the year .</t>
+          <t>coppola's directorial debut is an incredibly layered and stylistic film that , despite a fairly slow paced , almost humdrum approach to character development , still manages at least a decent attempt at meaningful cinema .</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>uplifting document worst possibilities mankind , among best films year .</t>
+          <t>coppolas directorial debut incredibly layered stylistic despite fairly slow paced almost humdrum approach character development still manages least decent attempt meaningful cinema</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -1654,11 +1654,11 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>1953</v>
+        <v>1987</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>coppola's directorial debut is an incredibly layered and stylistic film that , despite a fairly slow paced , almost humdrum approach to character development , still manages at least a decent attempt at meaningful cinema .</t>
+          <t>methodical , measured , and gently tedious in its comedy , secret ballot is a purposefully reductive movie -- which may be why it's so successful at lodging itself in the brain .</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>coppola 's directorial debut incredibly layered stylistic , despite fairly slow paced , almost humdrum approach character development , still manages least decent attempt meaningful cinema .</t>
+          <t>methodical measured gently tedious comedy secret ballot purposefully reductive may successful lodging brain</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -1675,11 +1675,11 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>1987</v>
+        <v>2029</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>methodical , measured , and gently tedious in its comedy , secret ballot is a purposefully reductive movie -- which may be why it's so successful at lodging itself in the brain .</t>
+          <t>" red dragon " is entertaining . an obvious copy of one of the best films ever made , how could it not be ? but it is entertaining on an inferior level . it is a popcorn film , not a must-own , or even a must-see .</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>methodical , measured , gently tedious comedy , secret ballot purposefully reductive -- may 's successful lodging brain .</t>
+          <t>red dragon entertaining obvious copy best films ever made could entertaining inferior level popcorn mustown even mustsee</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -1696,11 +1696,11 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>2029</v>
+        <v>2046</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>" red dragon " is entertaining . an obvious copy of one of the best films ever made , how could it not be ? but it is entertaining on an inferior level . it is a popcorn film , not a must-own , or even a must-see .</t>
+          <t>a disturbing examination of what appears to be the definition of a 'bad' police shooting .</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>`` red dragon `` entertaining . obvious copy best films ever made , could ? entertaining inferior level . popcorn , must-own , even must-see .</t>
+          <t>disturbing examination appears definition bad police shooting</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -1717,11 +1717,11 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>2046</v>
+        <v>2104</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>a disturbing examination of what appears to be the definition of a 'bad' police shooting .</t>
+          <t>at its worst the screenplay is callow , but at its best it is a young artist's thoughtful consideration of fatherhood .</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1729,7 +1729,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>disturbing examination appears definition 'bad ' police shooting .</t>
+          <t>worst screenplay callow best young artists thoughtful consideration fatherhood</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -1738,11 +1738,11 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>2104</v>
+        <v>2116</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>at its worst the screenplay is callow , but at its best it is a young artist's thoughtful consideration of fatherhood .</t>
+          <t>light-years ahead of paint-by-number american blockbusters like pearl harbor , at least artistically .</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>worst screenplay callow , best young artist 's thoughtful consideration fatherhood .</t>
+          <t>lightyears ahead paintbynumber american blockbusters pearl harbor least artistically</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -1759,11 +1759,11 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>2116</v>
+        <v>2216</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>light-years ahead of paint-by-number american blockbusters like pearl harbor , at least artistically .</t>
+          <t>i'm sure mainstream audiences will be baffled , but , for those with at least a minimal appreciation of woolf and clarissa dalloway , the hours represents two of those well spent .</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>light-years ahead paint-by-number american blockbusters pearl harbor , least artistically .</t>
+          <t>im sure mainstream audiences baffled least minimal appreciation woolf clarissa dalloway hours represents two well spent</t>
         </is>
       </c>
       <c r="E64" t="n">
@@ -1780,11 +1780,11 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>2216</v>
+        <v>2232</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>i'm sure mainstream audiences will be baffled , but , for those with at least a minimal appreciation of woolf and clarissa dalloway , the hours represents two of those well spent .</t>
+          <t>while insomnia is in many ways a conventional , even predictable remake , nolan's penetrating undercurrent of cerebral and cinemantic flair lends ( it ) stimulating depth .</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>'m sure mainstream audiences baffled , , least minimal appreciation woolf clarissa dalloway , hours represents two well spent .</t>
+          <t>insomnia ways conventional even predictable remake nolans penetrating undercurrent cerebral cinemantic flair lends stimulating depth</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -1801,11 +1801,11 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>2232</v>
+        <v>2258</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>while insomnia is in many ways a conventional , even predictable remake , nolan's penetrating undercurrent of cerebral and cinemantic flair lends ( it ) stimulating depth .</t>
+          <t>you just know something terrible is going to happen . but when it does , you're entirely unprepared .</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>insomnia ways conventional , even predictable remake , nolan 's penetrating undercurrent cerebral cinemantic flair lends ( ) stimulating depth .</t>
+          <t>know something terrible going happen youre entirely unprepared</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -1822,11 +1822,11 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>2258</v>
+        <v>2267</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>you just know something terrible is going to happen . but when it does , you're entirely unprepared .</t>
+          <t>the film is predictable in the reassuring manner of a beautifully sung holiday carol .</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>know something terrible going happen . , 're entirely unprepared .</t>
+          <t>predictable reassuring manner beautifully sung holiday carol</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -1843,11 +1843,11 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>2267</v>
+        <v>2283</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>the film is predictable in the reassuring manner of a beautifully sung holiday carol .</t>
+          <t>although it includes a fair share of dumb drug jokes and predictable slapstick , " orange county " is far funnier than it would seem to have any right to be .</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>predictable reassuring manner beautifully sung holiday carol .</t>
+          <t>although includes fair share dumb drug jokes predictable slapstick orange county far funnier would seem right</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -1864,11 +1864,11 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>2283</v>
+        <v>2302</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>although it includes a fair share of dumb drug jokes and predictable slapstick , " orange county " is far funnier than it would seem to have any right to be .</t>
+          <t>the stripped-down dramatic constructs , austere imagery and abstract characters are equal parts poetry and politics , obvious at times but evocative and heartfelt .</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>although includes fair share dumb drug jokes predictable slapstick , `` orange county `` far funnier would seem right .</t>
+          <t>strippeddown dramatic constructs austere imagery abstract characters equal parts poetry politics obvious times evocative heartfelt</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -1885,11 +1885,11 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>2302</v>
+        <v>2313</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>the stripped-down dramatic constructs , austere imagery and abstract characters are equal parts poetry and politics , obvious at times but evocative and heartfelt .</t>
+          <t>a different movie -- sometimes tedious -- by a director many viewers would like to skip but film buffs should get to know .</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>stripped-down dramatic constructs , austere imagery abstract characters equal parts poetry politics , obvious times evocative heartfelt .</t>
+          <t>different sometimes tedious director viewers would skip buffs get know</t>
         </is>
       </c>
       <c r="E70" t="n">
@@ -1906,11 +1906,11 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>2313</v>
+        <v>2334</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>a different movie -- sometimes tedious -- by a director many viewers would like to skip but film buffs should get to know .</t>
+          <t>the premise of jason x is silly but strangely believable .</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1918,7 +1918,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>different -- sometimes tedious -- director viewers would skip buffs get know .</t>
+          <t>premise jason x silly strangely believable</t>
         </is>
       </c>
       <c r="E71" t="n">
@@ -1927,11 +1927,11 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>2334</v>
+        <v>2345</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>the premise of jason x is silly but strangely believable .</t>
+          <t>triple x is a double agent , and he's one bad dude . when you've got the wildly popular vin diesel in the equation , it adds up to big box office bucks all but guaranteed .</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1939,7 +1939,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>premise jason x silly strangely believable .</t>
+          <t>triple x double agent hes bad dude youve got wildly popular vin diesel equation adds big box office bucks guaranteed</t>
         </is>
       </c>
       <c r="E72" t="n">
@@ -1948,11 +1948,11 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>2345</v>
+        <v>2382</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>triple x is a double agent , and he's one bad dude . when you've got the wildly popular vin diesel in the equation , it adds up to big box office bucks all but guaranteed .</t>
+          <t>a movie that's just plain awful but still manages to entertain on a guilty-pleasure , so-bad-it's-funny level .</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>triple x double agent , 's bad dude . 've got wildly popular vin diesel equation , adds big box office bucks guaranteed .</t>
+          <t>thats plain awful still manages entertain guiltypleasure sobaditsfunny level</t>
         </is>
       </c>
       <c r="E73" t="n">
@@ -1969,11 +1969,11 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>2382</v>
+        <v>2387</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>a movie that's just plain awful but still manages to entertain on a guilty-pleasure , so-bad-it's-funny level .</t>
+          <t>this odd , distant portuguese import more or less borrows from bad lieutenant and les vampires , and comes up with a kind of art-house gay porn film .</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>'s plain awful still manages entertain guilty-pleasure , so-bad-it's-funny level .</t>
+          <t>odd distant portuguese import less borrows bad lieutenant les vampires comes kind arthouse gay porn</t>
         </is>
       </c>
       <c r="E74" t="n">
@@ -1990,11 +1990,11 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>2387</v>
+        <v>2415</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>this odd , distant portuguese import more or less borrows from bad lieutenant and les vampires , and comes up with a kind of art-house gay porn film .</t>
+          <t>at times a bit melodramatic and even a little dated ( depending upon where you live ) , ignorant fairies is still quite good-natured and not a bad way to spend an hour or two .</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>odd , distant portuguese import less borrows bad lieutenant les vampires , comes kind art-house gay porn .</t>
+          <t>times bit melodramatic even dated depending upon live ignorant fairies still quite goodnatured bad way spend hour two</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -2011,11 +2011,11 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>2415</v>
+        <v>2436</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>at times a bit melodramatic and even a little dated ( depending upon where you live ) , ignorant fairies is still quite good-natured and not a bad way to spend an hour or two .</t>
+          <t>wickedly funny , visually engrossing , never boring , this movie challenges us to think about the ways we consume pop culture .</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>times bit melodramatic even dated ( depending upon live ) , ignorant fairies still quite good-natured bad way spend hour two .</t>
+          <t>wickedly visually engrossing never boring challenges us think ways consume pop culture</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -2032,11 +2032,11 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>2436</v>
+        <v>2484</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>wickedly funny , visually engrossing , never boring , this movie challenges us to think about the ways we consume pop culture .</t>
+          <t>it's truly awful and heartbreaking subject matter , but one whose lessons are well worth revisiting as many times as possible .</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -2044,7 +2044,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>wickedly , visually engrossing , never boring , challenges us think ways consume pop culture .</t>
+          <t>truly awful heartbreaking subject matter whose lessons well worth revisiting times possible</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -2053,11 +2053,11 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>2484</v>
+        <v>2485</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>it's truly awful and heartbreaking subject matter , but one whose lessons are well worth revisiting as many times as possible .</t>
+          <t>though intrepid in exploring an attraction that crosses sexual identity , ozpetek falls short in showing us antonia's true emotions . . . but at the very least , his secret life will leave you thinking .</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>'s truly awful heartbreaking subject matter , whose lessons well worth revisiting times possible .</t>
+          <t>though intrepid exploring attraction crosses sexual identity ozpetek falls short showing us antonias true emotions least secret life leave thinking</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -2074,11 +2074,11 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>2485</v>
+        <v>2521</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>though intrepid in exploring an attraction that crosses sexual identity , ozpetek falls short in showing us antonia's true emotions . . . but at the very least , his secret life will leave you thinking .</t>
+          <t>although it doesn't always hang together -- violence and whimsy don't combine easily -- " cherish " certainly isn't dull .</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -2086,7 +2086,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>though intrepid exploring attraction crosses sexual identity , ozpetek falls short showing us antonia 's true emotions . . . least , secret life leave thinking .</t>
+          <t>although doesnt always hang together violence whimsy dont combine easily cherish certainly isnt dull</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2095,11 +2095,11 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>2521</v>
+        <v>2562</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>although it doesn't always hang together -- violence and whimsy don't combine easily -- " cherish " certainly isn't dull .</t>
+          <t>this may be dover kosashvili's feature directing debut , but it looks an awful lot like life -- gritty , awkward and ironic .</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>although n't always hang together -- violence whimsy n't combine easily -- `` cherish `` certainly n't dull .</t>
+          <t>may dover kosashvilis feature directing debut looks awful lot life gritty awkward ironic</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -2116,11 +2116,11 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>2562</v>
+        <v>2582</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>this may be dover kosashvili's feature directing debut , but it looks an awful lot like life -- gritty , awkward and ironic .</t>
+          <t>not a bad choice here , assuming that . . . the air-conditioning in the theater is working properly .</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>may dover kosashvili 's feature directing debut , looks awful lot life -- gritty , awkward ironic .</t>
+          <t>bad choice assuming airconditioning theater working properly</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -2137,11 +2137,11 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>2582</v>
+        <v>2609</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>not a bad choice here , assuming that . . . the air-conditioning in the theater is working properly .</t>
+          <t>a wild ride juiced with enough energy and excitement for at least three films .</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>bad choice , assuming . . . air-conditioning theater working properly .</t>
+          <t>wild ride juiced energy excitement least three films</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -2158,11 +2158,11 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>2609</v>
+        <v>2612</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>a wild ride juiced with enough energy and excitement for at least three films .</t>
+          <t>the movie is not as terrible as the synergistic impulse that created it .</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -2170,7 +2170,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>wild ride juiced energy excitement least three films .</t>
+          <t>terrible synergistic impulse created</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -2179,11 +2179,11 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>2612</v>
+        <v>2613</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>the movie is not as terrible as the synergistic impulse that created it .</t>
+          <t>a typically observant , carefully nuanced and intimate french coming-of-age film that is an encouraging debut feature but has a needlessly downbeat ending that is too heavy for all that has preceded it .</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>terrible synergistic impulse created .</t>
+          <t>typically observant carefully nuanced intimate french comingofage encouraging debut feature needlessly downbeat ending heavy preceded</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -2200,11 +2200,11 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>2613</v>
+        <v>2637</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>a typically observant , carefully nuanced and intimate french coming-of-age film that is an encouraging debut feature but has a needlessly downbeat ending that is too heavy for all that has preceded it .</t>
+          <t>offers big , fat , dumb laughs that may make you hate yourself for giving in . ah , what the hell .</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -2212,7 +2212,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>typically observant , carefully nuanced intimate french coming-of-age encouraging debut feature needlessly downbeat ending heavy preceded .</t>
+          <t>offers big fat dumb laughs may hate giving ah hell</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -2221,11 +2221,11 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>2637</v>
+        <v>2654</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>offers big , fat , dumb laughs that may make you hate yourself for giving in . ah , what the hell .</t>
+          <t>murderous maids has a lot going for it , not least the brilliant performances by testud . . . and parmentier .</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>offers big , fat , dumb laughs may hate giving . ah , hell .</t>
+          <t>murderous maids lot going least brilliant performances testud parmentier</t>
         </is>
       </c>
       <c r="E86" t="n">
@@ -2242,11 +2242,11 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>2654</v>
+        <v>2657</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>murderous maids has a lot going for it , not least the brilliant performances by testud . . . and parmentier .</t>
+          <t>it's light on the chills and heavy on the atmospheric weirdness , and there are moments of jaw-droppingly odd behavior -- yet i found it weirdly appealing .</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -2254,7 +2254,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>murderous maids lot going , least brilliant performances testud . . . parmentier .</t>
+          <t>light chills heavy atmospheric weirdness moments jawdroppingly odd behavior yet found weirdly appealing</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -2263,11 +2263,11 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>2657</v>
+        <v>2725</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>it's light on the chills and heavy on the atmospheric weirdness , and there are moments of jaw-droppingly odd behavior -- yet i found it weirdly appealing .</t>
+          <t>[moore's] better at fingering problems than finding solutions . but though he only scratches the surface , at least he provides a strong itch to explore more .</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>'s light chills heavy atmospheric weirdness , moments jaw-droppingly odd behavior -- yet found weirdly appealing .</t>
+          <t>moores better fingering problems finding solutions though scratches surface least provides strong itch explore</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -2284,11 +2284,11 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>2725</v>
+        <v>2731</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[moore's] better at fingering problems than finding solutions . but though he only scratches the surface , at least he provides a strong itch to explore more .</t>
+          <t>vincent gallo is right at home in this french shocker playing his usual bad boy weirdo role .</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -2296,7 +2296,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>[ moore 's ] better fingering problems finding solutions . though scratches surface , least provides strong itch explore .</t>
+          <t>vincent gallo right home french shocker playing usual bad boy weirdo role</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -2305,11 +2305,11 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>2731</v>
+        <v>2804</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>vincent gallo is right at home in this french shocker playing his usual bad boy weirdo role .</t>
+          <t>this starts off with a 1950's doris day feel and it gets very ugly , very fast . the first five minutes will have you talking 'til the end of the year !</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -2317,7 +2317,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>vincent gallo right home french shocker playing usual bad boy weirdo role .</t>
+          <t>starts doris day feel gets ugly fast first five minutes talking til end year</t>
         </is>
       </c>
       <c r="E90" t="n">
@@ -2326,11 +2326,11 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>2804</v>
+        <v>2805</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>this starts off with a 1950's doris day feel and it gets very ugly , very fast . the first five minutes will have you talking 'til the end of the year !</t>
+          <t>triumph of love is a very silly movie , but the silliness has a pedigree .</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>starts 1950 's doris day feel gets ugly , fast . first five minutes talking 'til end year !</t>
+          <t>triumph love silly silliness pedigree</t>
         </is>
       </c>
       <c r="E91" t="n">
@@ -2347,11 +2347,11 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>2805</v>
+        <v>2910</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>triumph of love is a very silly movie , but the silliness has a pedigree .</t>
+          <t>the quiet american isn't a bad film , it's just one that could easily wait for your pay per view dollar .</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>triumph love silly , silliness pedigree .</t>
+          <t>quiet american isnt bad could easily wait pay per view dollar</t>
         </is>
       </c>
       <c r="E92" t="n">
@@ -2368,11 +2368,11 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>2910</v>
+        <v>2965</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>the quiet american isn't a bad film , it's just one that could easily wait for your pay per view dollar .</t>
+          <t>originality ain't on the menu , but there's never a dull moment in the giant spider invasion comic chiller .</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -2380,7 +2380,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>quiet american n't bad , 's could easily wait pay per view dollar .</t>
+          <t>originality aint menu theres never dull moment giant spider invasion comic chiller</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -2389,11 +2389,11 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>2965</v>
+        <v>2972</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>originality ain't on the menu , but there's never a dull moment in the giant spider invasion comic chiller .</t>
+          <t>while the now 72-year-old robert evans been slowed down by a stroke , he has at least one more story to tell : his own .</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>originality ai n't menu , 's never dull moment giant spider invasion comic chiller .</t>
+          <t>yearold robert evans slowed stroke least story tell</t>
         </is>
       </c>
       <c r="E94" t="n">
@@ -2410,11 +2410,11 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>2972</v>
+        <v>3009</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>while the now 72-year-old robert evans been slowed down by a stroke , he has at least one more story to tell : his own .</t>
+          <t>halloween : resurrection isn't exactly quality cinema , but it isn't nearly as terrible as it cold have been .</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -2422,7 +2422,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>72-year-old robert evans slowed stroke , least story tell : .</t>
+          <t>halloween resurrection isnt exactly quality cinema isnt nearly terrible cold</t>
         </is>
       </c>
       <c r="E95" t="n">
@@ -2431,11 +2431,11 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>3009</v>
+        <v>3077</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>halloween : resurrection isn't exactly quality cinema , but it isn't nearly as terrible as it cold have been .</t>
+          <t>it's not the least of afghan tragedies that this noble warlord would be consigned to the dustbin of history .</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -2443,7 +2443,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>halloween : resurrection n't exactly quality cinema , n't nearly terrible cold .</t>
+          <t>least afghan tragedies noble warlord would consigned dustbin history</t>
         </is>
       </c>
       <c r="E96" t="n">
@@ -2452,11 +2452,11 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>3077</v>
+        <v>3137</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>it's not the least of afghan tragedies that this noble warlord would be consigned to the dustbin of history .</t>
+          <t>with lesser talents , high crimes would be entertaining , but forgettable . with freeman and judd , i'll at least remember their characters .</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -2464,7 +2464,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>'s least afghan tragedies noble warlord would consigned dustbin history .</t>
+          <t>lesser talents high crimes would entertaining forgettable freeman judd ill least remember characters</t>
         </is>
       </c>
       <c r="E97" t="n">
@@ -2473,11 +2473,11 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>3137</v>
+        <v>3146</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>with lesser talents , high crimes would be entertaining , but forgettable . with freeman and judd , i'll at least remember their characters .</t>
+          <t>i don't feel the least bit ashamed in admitting that my enjoyment came at the expense of seeing justice served , even if it's a dish that's best served cold .</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -2485,7 +2485,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>lesser talents , high crimes would entertaining , forgettable . freeman judd , 'll least remember characters .</t>
+          <t>dont feel least bit ashamed admitting enjoyment came expense seeing justice served even dish thats best served cold</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -2494,11 +2494,11 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>3146</v>
+        <v>3150</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>i don't feel the least bit ashamed in admitting that my enjoyment came at the expense of seeing justice served , even if it's a dish that's best served cold .</t>
+          <t>because eight legged freaks is partly an homage to them , tarantula and other low- budget b-movie thrillers of the 1950s and '60s , the movie is a silly ( but not sophomoric ) romp through horror and hellish conditions .</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>n't feel least bit ashamed admitting enjoyment came expense seeing justice served , even 's dish 's best served cold .</t>
+          <t>eight legged freaks partly homage tarantula low budget bmovie thrillers silly sophomoric romp horror hellish conditions</t>
         </is>
       </c>
       <c r="E99" t="n">
@@ -2515,11 +2515,11 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>3150</v>
+        <v>3197</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>because eight legged freaks is partly an homage to them , tarantula and other low- budget b-movie thrillers of the 1950s and '60s , the movie is a silly ( but not sophomoric ) romp through horror and hellish conditions .</t>
+          <t>it's never dull and always looks good .</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -2527,7 +2527,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>eight legged freaks partly homage , tarantula low- budget b-movie thrillers 1950s '60s , silly ( sophomoric ) romp horror hellish conditions .</t>
+          <t>never dull always looks</t>
         </is>
       </c>
       <c r="E100" t="n">
@@ -2536,11 +2536,11 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>3197</v>
+        <v>3234</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>it's never dull and always looks good .</t>
+          <t>despite its old-hat set-up and predictable plot , empire still has enough moments to keep it entertaining .</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>'s never dull always looks .</t>
+          <t>despite oldhat setup predictable plot empire still moments keep entertaining</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -2557,11 +2557,11 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>3234</v>
+        <v>3308</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>despite its old-hat set-up and predictable plot , empire still has enough moments to keep it entertaining .</t>
+          <t>mr . deeds is , as comedy goes , very silly -- and in the best way .</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>despite old-hat set-up predictable plot , empire still moments keep entertaining .</t>
+          <t>mr deeds comedy goes silly best way</t>
         </is>
       </c>
       <c r="E102" t="n">
@@ -2578,11 +2578,11 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>3308</v>
+        <v>3331</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>mr . deeds is , as comedy goes , very silly -- and in the best way .</t>
+          <t>until its final minutes this is a perceptive study of two families in crisis -- and of two girls whose friendship is severely tested by bad luck and their own immaturity .</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -2590,7 +2590,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>mr . deeds , comedy goes , silly -- best way .</t>
+          <t>final minutes perceptive study two families crisis two girls whose friendship severely tested bad luck immaturity</t>
         </is>
       </c>
       <c r="E103" t="n">
@@ -2599,11 +2599,11 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>3331</v>
+        <v>3334</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>until its final minutes this is a perceptive study of two families in crisis -- and of two girls whose friendship is severely tested by bad luck and their own immaturity .</t>
+          <t>for all its problems . . . the lady and the duke surprisingly manages never to grow boring . . . which proves that rohmer still has a sense of his audience .</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -2611,7 +2611,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>final minutes perceptive study two families crisis -- two girls whose friendship severely tested bad luck immaturity .</t>
+          <t>problems lady duke surprisingly manages never grow boring proves rohmer still sense audience</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -2620,11 +2620,11 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>3334</v>
+        <v>3347</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>for all its problems . . . the lady and the duke surprisingly manages never to grow boring . . . which proves that rohmer still has a sense of his audience .</t>
+          <t>this is an extraordinary film , not least because it is japanese and yet feels universal .</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -2632,7 +2632,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>problems . . . lady duke surprisingly manages never grow boring . . . proves rohmer still sense audience .</t>
+          <t>extraordinary least japanese yet feels universal</t>
         </is>
       </c>
       <c r="E105" t="n">
@@ -2641,11 +2641,11 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>3347</v>
+        <v>3364</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>this is an extraordinary film , not least because it is japanese and yet feels universal .</t>
+          <t>despite the predictable parent vs . child coming-of-age theme , first-class , natural acting and a look at " the real americans " make this a charmer .</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -2653,7 +2653,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>extraordinary , least japanese yet feels universal .</t>
+          <t>despite predictable parent vs child comingofage theme firstclass natural acting look real americans charmer</t>
         </is>
       </c>
       <c r="E106" t="n">
@@ -2662,11 +2662,11 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>3364</v>
+        <v>3386</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>despite the predictable parent vs . child coming-of-age theme , first-class , natural acting and a look at " the real americans " make this a charmer .</t>
+          <t>the movie plays up the cartoon's more obvious strength of snazziness while neglecting its less conspicuous writing strength .</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2674,7 +2674,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>despite predictable parent vs . child coming-of-age theme , first-class , natural acting look `` real americans `` charmer .</t>
+          <t>plays cartoons obvious strength snazziness neglecting less conspicuous writing strength</t>
         </is>
       </c>
       <c r="E107" t="n">
@@ -2683,11 +2683,11 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>3386</v>
+        <v>3413</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>the movie plays up the cartoon's more obvious strength of snazziness while neglecting its less conspicuous writing strength .</t>
+          <t>it's got some pretentious eye-rolling moments and it didn't entirely grab me , but there's stuff here to like .</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -2695,7 +2695,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>plays cartoon 's obvious strength snazziness neglecting less conspicuous writing strength .</t>
+          <t>got pretentious eyerolling moments didnt entirely grab theres stuff</t>
         </is>
       </c>
       <c r="E108" t="n">
@@ -2704,11 +2704,11 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>3413</v>
+        <v>3513</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>it's got some pretentious eye-rolling moments and it didn't entirely grab me , but there's stuff here to like .</t>
+          <t>there aren't too many films that can be as simultaneously funny , offbeat and heartwarming ( without a thick shmear of the goo , at least ) , but " elling " manages to do all three quite well , making it one of the year's most enjoyable releases .</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>'s got pretentious eye-rolling moments n't entirely grab , 's stuff .</t>
+          <t>arent films simultaneously offbeat heartwarming without thick shmear goo least elling manages three quite well making years enjoyable releases</t>
         </is>
       </c>
       <c r="E109" t="n">
@@ -2725,11 +2725,11 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>3444</v>
+        <v>3525</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>earnest , unsubtle and hollywood-predictable , green dragon is still a deeply moving effort to put a human face on the travail of thousands of vietnamese .</t>
+          <t>a rock-solid gangster movie with a fair amount of suspense , intriguing characters and bizarre bank robberies , plus a heavy dose of father-and-son dynamics .</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -2737,7 +2737,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>earnest , unsubtle hollywood-predictable , green dragon still deeply moving effort put human face travail thousands vietnamese .</t>
+          <t>rocksolid gangster fair amount suspense intriguing characters bizarre bank robberies plus heavy dose fatherandson dynamics</t>
         </is>
       </c>
       <c r="E110" t="n">
@@ -2746,11 +2746,11 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>3511</v>
+        <v>3548</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>if you ignore the cliches and concentrate on city by the sea's interpersonal drama , it ain't half-bad .</t>
+          <t>it's not like having a real film of nijinsky , but at least it's better than that eponymous 1980 biopic that used soap in the places where the mysteries lingered .</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -2758,7 +2758,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>ignore cliches concentrate city sea 's interpersonal drama , ai n't half-bad .</t>
+          <t>real nijinsky least better eponymous biopic used soap places mysteries lingered</t>
         </is>
       </c>
       <c r="E111" t="n">
@@ -2767,11 +2767,11 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>3513</v>
+        <v>3591</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>there aren't too many films that can be as simultaneously funny , offbeat and heartwarming ( without a thick shmear of the goo , at least ) , but " elling " manages to do all three quite well , making it one of the year's most enjoyable releases .</t>
+          <t>i don't know if frailty will turn bill paxton into an a-list director , but he can rest contentedly with the knowledge that he's made at least one damn fine horror movie .</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>n't films simultaneously , offbeat heartwarming ( without thick shmear goo , least ) , `` elling `` manages three quite well , making year 's enjoyable releases .</t>
+          <t>dont know frailty turn bill paxton alist director rest contentedly knowledge hes made least damn fine horror</t>
         </is>
       </c>
       <c r="E112" t="n">
@@ -2788,11 +2788,11 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>3525</v>
+        <v>3686</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>a rock-solid gangster movie with a fair amount of suspense , intriguing characters and bizarre bank robberies , plus a heavy dose of father-and-son dynamics .</t>
+          <t>from the dull , surreal ache of mortal awareness emerges a radiant character portrait .</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -2800,7 +2800,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>rock-solid gangster fair amount suspense , intriguing characters bizarre bank robberies , plus heavy dose father-and-son dynamics .</t>
+          <t>dull surreal ache mortal awareness emerges radiant character portrait</t>
         </is>
       </c>
       <c r="E113" t="n">
@@ -2809,11 +2809,11 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>3548</v>
+        <v>3688</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>it's not like having a real film of nijinsky , but at least it's better than that eponymous 1980 biopic that used soap in the places where the mysteries lingered .</t>
+          <t>it's not particularly subtle . . . however , it still manages to build to a terrifying , if obvious , conclusion .</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>'s real nijinsky , least 's better eponymous 1980 biopic used soap places mysteries lingered .</t>
+          <t>particularly subtle however still manages build terrifying obvious conclusion</t>
         </is>
       </c>
       <c r="E114" t="n">
@@ -2830,11 +2830,11 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>3591</v>
+        <v>3712</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>i don't know if frailty will turn bill paxton into an a-list director , but he can rest contentedly with the knowledge that he's made at least one damn fine horror movie .</t>
+          <t>sure , it's contrived and predictable , but its performances are so well tuned that the film comes off winningly , even though it's never as solid as you want it to be .</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -2842,7 +2842,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>n't know frailty turn bill paxton a-list director , rest contentedly knowledge 's made least damn fine horror .</t>
+          <t>sure contrived predictable performances well tuned comes winningly even though never solid want</t>
         </is>
       </c>
       <c r="E115" t="n">
@@ -2851,11 +2851,11 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>3686</v>
+        <v>3763</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>from the dull , surreal ache of mortal awareness emerges a radiant character portrait .</t>
+          <t>the film reminds me of a vastly improved germanic version of my big fat greek wedding -- with better characters , some genuine quirkiness and at least a measure of style . the difference is that i truly enjoyed most of mostly martha while i ne</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -2863,7 +2863,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>dull , surreal ache mortal awareness emerges radiant character portrait .</t>
+          <t>reminds vastly improved germanic version big fat greek wedding better characters genuine quirkiness least measure style difference truly enjoyed mostly martha ne</t>
         </is>
       </c>
       <c r="E116" t="n">
@@ -2872,11 +2872,11 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>3688</v>
+        <v>3873</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>it's not particularly subtle . . . however , it still manages to build to a terrifying , if obvious , conclusion .</t>
+          <t>with so many bad romances out there , this is the kind of movie that deserves a chance to shine .</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -2884,7 +2884,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>'s particularly subtle . . . however , still manages build terrifying , obvious , conclusion .</t>
+          <t>bad romances kind deserves chance shine</t>
         </is>
       </c>
       <c r="E117" t="n">
@@ -2893,11 +2893,11 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>3712</v>
+        <v>3890</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>sure , it's contrived and predictable , but its performances are so well tuned that the film comes off winningly , even though it's never as solid as you want it to be .</t>
+          <t>the result is somewhat satisfying -- it still comes from spielberg , who has never made anything that wasn't at least watchable . but it's also disappointing to a certain degree .</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -2905,7 +2905,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>sure , 's contrived predictable , performances well tuned comes winningly , even though 's never solid want .</t>
+          <t>result somewhat satisfying still comes spielberg never made anything wasnt least watchable also disappointing certain degree</t>
         </is>
       </c>
       <c r="E118" t="n">
@@ -2914,11 +2914,11 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>3763</v>
+        <v>4014</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>the film reminds me of a vastly improved germanic version of my big fat greek wedding -- with better characters , some genuine quirkiness and at least a measure of style . the difference is that i truly enjoyed most of mostly martha while i ne</t>
+          <t>the actresses find their own rhythm and protect each other from the script's bad ideas and awkwardness .</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -2926,7 +2926,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>reminds vastly improved germanic version big fat greek wedding -- better characters , genuine quirkiness least measure style . difference truly enjoyed mostly martha ne</t>
+          <t>actresses find rhythm protect scripts bad ideas awkwardness</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -2935,11 +2935,11 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>3873</v>
+        <v>4033</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>with so many bad romances out there , this is the kind of movie that deserves a chance to shine .</t>
+          <t>while the plot follows a predictable connect-the-dots course . . . director john schultz colors the picture in some evocative shades .</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -2947,7 +2947,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>bad romances , kind deserves chance shine .</t>
+          <t>plot follows predictable connectthedots course director john schultz colors picture evocative shades</t>
         </is>
       </c>
       <c r="E120" t="n">
@@ -2956,11 +2956,11 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>3890</v>
+        <v>4047</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>the result is somewhat satisfying -- it still comes from spielberg , who has never made anything that wasn't at least watchable . but it's also disappointing to a certain degree .</t>
+          <t>yes , mibii is rote work and predictable , but with a philosophical visual coming right at the end that extravagantly redeems it .</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2968,7 +2968,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>result somewhat satisfying -- still comes spielberg , never made anything n't least watchable . 's also disappointing certain degree .</t>
+          <t>yes mibii rote work predictable philosophical visual coming right end extravagantly redeems</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -2977,11 +2977,11 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>4014</v>
+        <v>4077</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>the actresses find their own rhythm and protect each other from the script's bad ideas and awkwardness .</t>
+          <t>scotland looks wonderful , the fans are often funny fanatics , the showdown sure beats a bad day of golf .</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2989,7 +2989,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>actresses find rhythm protect script 's bad ideas awkwardness .</t>
+          <t>scotland looks wonderful fans often fanatics showdown sure beats bad day golf</t>
         </is>
       </c>
       <c r="E122" t="n">
@@ -2998,11 +2998,11 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>4033</v>
+        <v>4108</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>while the plot follows a predictable connect-the-dots course . . . director john schultz colors the picture in some evocative shades .</t>
+          <t>while not all that bad of a movie , it's nowhere near as good as the original .</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -3010,7 +3010,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>plot follows predictable connect-the-dots course . . . director john schultz colors picture evocative shades .</t>
+          <t>bad nowhere near original</t>
         </is>
       </c>
       <c r="E123" t="n">
@@ -3019,11 +3019,11 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>4047</v>
+        <v>4139</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>yes , mibii is rote work and predictable , but with a philosophical visual coming right at the end that extravagantly redeems it .</t>
+          <t>jackson tries to keep the plates spinning as best he can , but all the bouncing back and forth can't help but become a bit tedious -- even with the breathtaking landscapes and villainous varmints there to distract you from the ricocheting .</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -3031,7 +3031,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>yes , mibii rote work predictable , philosophical visual coming right end extravagantly redeems .</t>
+          <t>jackson tries keep plates spinning best bouncing back forth cant help become bit tedious even breathtaking landscapes villainous varmints distract ricocheting</t>
         </is>
       </c>
       <c r="E124" t="n">
@@ -3040,11 +3040,11 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>4077</v>
+        <v>4181</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>scotland looks wonderful , the fans are often funny fanatics , the showdown sure beats a bad day of golf .</t>
+          <t>seems based on ugly ideas instead of ugly behavior , as happiness was . . . hence , storytelling is far more appealing .</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -3052,7 +3052,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>scotland looks wonderful , fans often fanatics , showdown sure beats bad day golf .</t>
+          <t>seems based ugly ideas instead ugly behavior happiness hence storytelling far appealing</t>
         </is>
       </c>
       <c r="E125" t="n">
@@ -3061,11 +3061,11 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>4108</v>
+        <v>4183</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>while not all that bad of a movie , it's nowhere near as good as the original .</t>
+          <t>an intelligently made ( and beautifully edited ) picture that at the very least has a spark of life to it -- more than you can say for plenty of movies that flow through the hollywood pipeline without a hitch .</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -3073,7 +3073,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>bad , 's nowhere near original .</t>
+          <t>intelligently made beautifully edited picture least spark life say plenty movies flow hollywood pipeline without hitch</t>
         </is>
       </c>
       <c r="E126" t="n">
@@ -3082,11 +3082,11 @@
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>4139</v>
+        <v>4230</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>jackson tries to keep the plates spinning as best he can , but all the bouncing back and forth can't help but become a bit tedious -- even with the breathtaking landscapes and villainous varmints there to distract you from the ricocheting .</t>
+          <t>as the princess , sorvino glides gracefully from male persona to female without missing a beat . ben kingsley is truly funny , playing a kind of ghandi gone bad .</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -3094,7 +3094,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>jackson tries keep plates spinning best , bouncing back forth ca n't help become bit tedious -- even breathtaking landscapes villainous varmints distract ricocheting .</t>
+          <t>princess sorvino glides gracefully male persona female without missing beat ben kingsley truly playing kind ghandi gone bad</t>
         </is>
       </c>
       <c r="E127" t="n">
@@ -3103,11 +3103,11 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>4181</v>
+        <v>4235</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>seems based on ugly ideas instead of ugly behavior , as happiness was . . . hence , storytelling is far more appealing .</t>
+          <t>ranges from laugh-out-loud hilarious to wonder-what- time-it-is tedious .</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -3115,73 +3115,10 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>seems based ugly ideas instead ugly behavior , happiness . . . hence , storytelling far appealing .</t>
+          <t>ranges laughoutloud hilarious wonderwhat timeitis tedious</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="1" t="n">
-        <v>4183</v>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>an intelligently made ( and beautifully edited ) picture that at the very least has a spark of life to it -- more than you can say for plenty of movies that flow through the hollywood pipeline without a hitch .</t>
-        </is>
-      </c>
-      <c r="C129" t="n">
-        <v>1</v>
-      </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>intelligently made ( beautifully edited ) picture least spark life -- say plenty movies flow hollywood pipeline without hitch .</t>
-        </is>
-      </c>
-      <c r="E129" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="n">
-        <v>4230</v>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>as the princess , sorvino glides gracefully from male persona to female without missing a beat . ben kingsley is truly funny , playing a kind of ghandi gone bad .</t>
-        </is>
-      </c>
-      <c r="C130" t="n">
-        <v>1</v>
-      </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>princess , sorvino glides gracefully male persona female without missing beat . ben kingsley truly , playing kind ghandi gone bad .</t>
-        </is>
-      </c>
-      <c r="E130" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="n">
-        <v>4235</v>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>ranges from laugh-out-loud hilarious to wonder-what- time-it-is tedious .</t>
-        </is>
-      </c>
-      <c r="C131" t="n">
-        <v>1</v>
-      </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>ranges laugh-out-loud hilarious wonder-what- time-it-is tedious .</t>
-        </is>
-      </c>
-      <c r="E131" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>